<commit_message>
Clean Mode logic Done
</commit_message>
<xml_diff>
--- a/Modbus_Tags.xlsb.xlsx
+++ b/Modbus_Tags.xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dunca\Documents\GitHub\Alchemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B414792-0E83-4F92-A24A-DDA5C022DD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FA4A1F-E9E5-49F1-8C2F-DED9A3261558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{4AD5CBED-8372-44A8-B2C4-3A6BCD43FD21}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="173">
   <si>
     <t>Data Type</t>
   </si>
@@ -426,9 +426,6 @@
     <t>Access screen</t>
   </si>
   <si>
-    <t>Timer</t>
-  </si>
-  <si>
     <t>MB_HR[11]</t>
   </si>
   <si>
@@ -553,6 +550,15 @@
   </si>
   <si>
     <t>None/Blank</t>
+  </si>
+  <si>
+    <t>MB_HR[12]</t>
+  </si>
+  <si>
+    <t>TimerMin</t>
+  </si>
+  <si>
+    <t>TimerSec</t>
   </si>
 </sst>
 </file>
@@ -689,13 +695,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85483887-8404-42FC-A14C-0D59A783FB69}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E36:E37"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,7 +1327,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>24</v>
@@ -1525,7 +1531,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>128</v>
+        <v>172</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>31</v>
@@ -1537,7 +1543,24 @@
         <v>412</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>413</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1567,175 +1590,175 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" s="6"/>
     </row>
@@ -1760,10 +1783,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1822,10 +1845,10 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1868,10 +1891,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="12"/>
+      <c r="B17" s="13"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -1938,10 +1961,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B27" s="12"/>
+      <c r="A27" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="13"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -1956,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1978,37 +2001,37 @@
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+      <c r="A33" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+      <c r="A34" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
+      <c r="A35" s="12">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
+      <c r="A36" s="12">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
+      <c r="A37" s="12">
         <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14">
+      <c r="A38" s="12">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
+      <c r="A39" s="12">
         <v>10</v>
       </c>
     </row>
@@ -2100,12 +2123,12 @@
       <c r="A1" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2145,12 +2168,12 @@
       <c r="A4" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2194,12 +2217,12 @@
       <c r="A11" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>